<commit_message>
add columns in excel files to simplify
</commit_message>
<xml_diff>
--- a/raw_data/departementales_2021_t1.xlsx
+++ b/raw_data/departementales_2021_t1.xlsx
@@ -1236,7 +1236,7 @@
       <c r="DB2" t="inlineStr"/>
       <c r="DC2" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
       <c r="DB3" t="inlineStr"/>
       <c r="DC3" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -1786,7 +1786,7 @@
       <c r="DB4" t="inlineStr"/>
       <c r="DC4" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -2061,7 +2061,7 @@
       <c r="DB5" t="inlineStr"/>
       <c r="DC5" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -2336,7 +2336,7 @@
       <c r="DB6" t="inlineStr"/>
       <c r="DC6" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -2611,7 +2611,7 @@
       <c r="DB7" t="inlineStr"/>
       <c r="DC7" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -2886,7 +2886,7 @@
       <c r="DB8" t="inlineStr"/>
       <c r="DC8" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -3161,7 +3161,7 @@
       <c r="DB9" t="inlineStr"/>
       <c r="DC9" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -3436,7 +3436,7 @@
       <c r="DB10" t="inlineStr"/>
       <c r="DC10" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -3711,7 +3711,7 @@
       <c r="DB11" t="inlineStr"/>
       <c r="DC11" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -3986,7 +3986,7 @@
       <c r="DB12" t="inlineStr"/>
       <c r="DC12" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -4261,7 +4261,7 @@
       <c r="DB13" t="inlineStr"/>
       <c r="DC13" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -4536,7 +4536,7 @@
       <c r="DB14" t="inlineStr"/>
       <c r="DC14" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -4811,7 +4811,7 @@
       <c r="DB15" t="inlineStr"/>
       <c r="DC15" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -5086,7 +5086,7 @@
       <c r="DB16" t="inlineStr"/>
       <c r="DC16" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -5361,7 +5361,7 @@
       <c r="DB17" t="inlineStr"/>
       <c r="DC17" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -5636,7 +5636,7 @@
       <c r="DB18" t="inlineStr"/>
       <c r="DC18" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -5911,7 +5911,7 @@
       <c r="DB19" t="inlineStr"/>
       <c r="DC19" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -6186,7 +6186,7 @@
       <c r="DB20" t="inlineStr"/>
       <c r="DC20" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -6461,7 +6461,7 @@
       <c r="DB21" t="inlineStr"/>
       <c r="DC21" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -6736,7 +6736,7 @@
       <c r="DB22" t="inlineStr"/>
       <c r="DC22" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -7011,7 +7011,7 @@
       <c r="DB23" t="inlineStr"/>
       <c r="DC23" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -7286,7 +7286,7 @@
       <c r="DB24" t="inlineStr"/>
       <c r="DC24" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -7561,7 +7561,7 @@
       <c r="DB25" t="inlineStr"/>
       <c r="DC25" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -7836,7 +7836,7 @@
       <c r="DB26" t="inlineStr"/>
       <c r="DC26" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -8111,7 +8111,7 @@
       <c r="DB27" t="inlineStr"/>
       <c r="DC27" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -8386,7 +8386,7 @@
       <c r="DB28" t="inlineStr"/>
       <c r="DC28" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -8661,7 +8661,7 @@
       <c r="DB29" t="inlineStr"/>
       <c r="DC29" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -8936,7 +8936,7 @@
       <c r="DB30" t="inlineStr"/>
       <c r="DC30" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -9211,7 +9211,7 @@
       <c r="DB31" t="inlineStr"/>
       <c r="DC31" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -9486,7 +9486,7 @@
       <c r="DB32" t="inlineStr"/>
       <c r="DC32" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -9761,7 +9761,7 @@
       <c r="DB33" t="inlineStr"/>
       <c r="DC33" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -10036,7 +10036,7 @@
       <c r="DB34" t="inlineStr"/>
       <c r="DC34" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -10311,7 +10311,7 @@
       <c r="DB35" t="inlineStr"/>
       <c r="DC35" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -10586,7 +10586,7 @@
       <c r="DB36" t="inlineStr"/>
       <c r="DC36" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -10861,7 +10861,7 @@
       <c r="DB37" t="inlineStr"/>
       <c r="DC37" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -11136,7 +11136,7 @@
       <c r="DB38" t="inlineStr"/>
       <c r="DC38" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -11411,7 +11411,7 @@
       <c r="DB39" t="inlineStr"/>
       <c r="DC39" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -11686,7 +11686,7 @@
       <c r="DB40" t="inlineStr"/>
       <c r="DC40" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -11961,7 +11961,7 @@
       <c r="DB41" t="inlineStr"/>
       <c r="DC41" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -12236,7 +12236,7 @@
       <c r="DB42" t="inlineStr"/>
       <c r="DC42" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -12511,7 +12511,7 @@
       <c r="DB43" t="inlineStr"/>
       <c r="DC43" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -12786,7 +12786,7 @@
       <c r="DB44" t="inlineStr"/>
       <c r="DC44" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -13061,7 +13061,7 @@
       <c r="DB45" t="inlineStr"/>
       <c r="DC45" t="inlineStr">
         <is>
-          <t>92002</t>
+          <t>92_002</t>
         </is>
       </c>
     </row>
@@ -13320,7 +13320,7 @@
       <c r="DB46" t="inlineStr"/>
       <c r="DC46" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -13579,7 +13579,7 @@
       <c r="DB47" t="inlineStr"/>
       <c r="DC47" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -13838,7 +13838,7 @@
       <c r="DB48" t="inlineStr"/>
       <c r="DC48" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -14097,7 +14097,7 @@
       <c r="DB49" t="inlineStr"/>
       <c r="DC49" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -14356,7 +14356,7 @@
       <c r="DB50" t="inlineStr"/>
       <c r="DC50" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -14615,7 +14615,7 @@
       <c r="DB51" t="inlineStr"/>
       <c r="DC51" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -14874,7 +14874,7 @@
       <c r="DB52" t="inlineStr"/>
       <c r="DC52" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -15133,7 +15133,7 @@
       <c r="DB53" t="inlineStr"/>
       <c r="DC53" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -15392,7 +15392,7 @@
       <c r="DB54" t="inlineStr"/>
       <c r="DC54" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -15651,7 +15651,7 @@
       <c r="DB55" t="inlineStr"/>
       <c r="DC55" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -15910,7 +15910,7 @@
       <c r="DB56" t="inlineStr"/>
       <c r="DC56" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -16169,7 +16169,7 @@
       <c r="DB57" t="inlineStr"/>
       <c r="DC57" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -16428,7 +16428,7 @@
       <c r="DB58" t="inlineStr"/>
       <c r="DC58" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -16687,7 +16687,7 @@
       <c r="DB59" t="inlineStr"/>
       <c r="DC59" t="inlineStr">
         <is>
-          <t>92014</t>
+          <t>92_014</t>
         </is>
       </c>
     </row>
@@ -16914,7 +16914,7 @@
       <c r="DB60" t="inlineStr"/>
       <c r="DC60" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -17141,7 +17141,7 @@
       <c r="DB61" t="inlineStr"/>
       <c r="DC61" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -17368,7 +17368,7 @@
       <c r="DB62" t="inlineStr"/>
       <c r="DC62" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -17595,7 +17595,7 @@
       <c r="DB63" t="inlineStr"/>
       <c r="DC63" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -17822,7 +17822,7 @@
       <c r="DB64" t="inlineStr"/>
       <c r="DC64" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -18049,7 +18049,7 @@
       <c r="DB65" t="inlineStr"/>
       <c r="DC65" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -18276,7 +18276,7 @@
       <c r="DB66" t="inlineStr"/>
       <c r="DC66" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -18503,7 +18503,7 @@
       <c r="DB67" t="inlineStr"/>
       <c r="DC67" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -18730,7 +18730,7 @@
       <c r="DB68" t="inlineStr"/>
       <c r="DC68" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -18957,7 +18957,7 @@
       <c r="DB69" t="inlineStr"/>
       <c r="DC69" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -19184,7 +19184,7 @@
       <c r="DB70" t="inlineStr"/>
       <c r="DC70" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -19411,7 +19411,7 @@
       <c r="DB71" t="inlineStr"/>
       <c r="DC71" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -19638,7 +19638,7 @@
       <c r="DB72" t="inlineStr"/>
       <c r="DC72" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -19865,7 +19865,7 @@
       <c r="DB73" t="inlineStr"/>
       <c r="DC73" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -20092,7 +20092,7 @@
       <c r="DB74" t="inlineStr"/>
       <c r="DC74" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -20319,7 +20319,7 @@
       <c r="DB75" t="inlineStr"/>
       <c r="DC75" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -20546,7 +20546,7 @@
       <c r="DB76" t="inlineStr"/>
       <c r="DC76" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -20773,7 +20773,7 @@
       <c r="DB77" t="inlineStr"/>
       <c r="DC77" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -21000,7 +21000,7 @@
       <c r="DB78" t="inlineStr"/>
       <c r="DC78" t="inlineStr">
         <is>
-          <t>92019</t>
+          <t>92_019</t>
         </is>
       </c>
     </row>
@@ -21227,7 +21227,7 @@
       <c r="DB79" t="inlineStr"/>
       <c r="DC79" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -21454,7 +21454,7 @@
       <c r="DB80" t="inlineStr"/>
       <c r="DC80" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -21681,7 +21681,7 @@
       <c r="DB81" t="inlineStr"/>
       <c r="DC81" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -21908,7 +21908,7 @@
       <c r="DB82" t="inlineStr"/>
       <c r="DC82" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -22135,7 +22135,7 @@
       <c r="DB83" t="inlineStr"/>
       <c r="DC83" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -22362,7 +22362,7 @@
       <c r="DB84" t="inlineStr"/>
       <c r="DC84" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -22589,7 +22589,7 @@
       <c r="DB85" t="inlineStr"/>
       <c r="DC85" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -22816,7 +22816,7 @@
       <c r="DB86" t="inlineStr"/>
       <c r="DC86" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -23043,7 +23043,7 @@
       <c r="DB87" t="inlineStr"/>
       <c r="DC87" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -23270,7 +23270,7 @@
       <c r="DB88" t="inlineStr"/>
       <c r="DC88" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -23497,7 +23497,7 @@
       <c r="DB89" t="inlineStr"/>
       <c r="DC89" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -23724,7 +23724,7 @@
       <c r="DB90" t="inlineStr"/>
       <c r="DC90" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -23951,7 +23951,7 @@
       <c r="DB91" t="inlineStr"/>
       <c r="DC91" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>
@@ -24178,7 +24178,7 @@
       <c r="DB92" t="inlineStr"/>
       <c r="DC92" t="inlineStr">
         <is>
-          <t>92071</t>
+          <t>92_071</t>
         </is>
       </c>
     </row>

</xml_diff>